<commit_message>
Use '.count' as placeholder instead of '_count'
</commit_message>
<xml_diff>
--- a/src/test/resources/example.xlsx
+++ b/src/test/resources/example.xlsx
@@ -130,7 +130,10 @@
     <t>继续（%1$s）</t>
   </si>
   <si>
-    <t>number_of_day_count</t>
+    <t>continue.count</t>
+  </si>
+  <si>
+    <t>number_of_day.count</t>
   </si>
   <si>
     <t>%1$d days remaining</t>
@@ -143,9 +146,6 @@
   </si>
   <si>
     <t>one day remaining</t>
-  </si>
-  <si>
-    <t>剩余1天</t>
   </si>
 </sst>
 </file>
@@ -1384,7 +1384,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J359"/>
+  <dimension ref="A1:J360"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1595,10 +1595,10 @@
         <v>39</v>
       </c>
       <c r="C10" t="s" s="2">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D10" t="s" s="6">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="4"/>
@@ -1612,13 +1612,13 @@
         <v>5</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s" s="2">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D11" t="s" s="6">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="4"/>
@@ -1628,9 +1628,15 @@
       <c r="J11" s="4"/>
     </row>
     <row r="12" ht="16.5" customHeight="1">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="A12" t="s" s="2">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="C12" t="s" s="2">
+        <v>44</v>
+      </c>
       <c r="D12" s="6"/>
       <c r="E12" s="2"/>
       <c r="F12" s="4"/>
@@ -1736,11 +1742,11 @@
       <c r="J20" s="4"/>
     </row>
     <row r="21" ht="16.5" customHeight="1">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="2"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
@@ -2185,11 +2191,11 @@
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
       <c r="E58" s="7"/>
-      <c r="F58" s="7"/>
-      <c r="G58" s="7"/>
-      <c r="H58" s="7"/>
-      <c r="I58" s="7"/>
-      <c r="J58" s="7"/>
+      <c r="F58" s="4"/>
+      <c r="G58" s="4"/>
+      <c r="H58" s="4"/>
+      <c r="I58" s="4"/>
+      <c r="J58" s="4"/>
     </row>
     <row r="59" ht="16.5" customHeight="1">
       <c r="A59" s="7"/>
@@ -2233,11 +2239,11 @@
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
       <c r="E62" s="7"/>
-      <c r="F62" s="4"/>
-      <c r="G62" s="4"/>
-      <c r="H62" s="4"/>
-      <c r="I62" s="4"/>
-      <c r="J62" s="4"/>
+      <c r="F62" s="7"/>
+      <c r="G62" s="7"/>
+      <c r="H62" s="7"/>
+      <c r="I62" s="7"/>
+      <c r="J62" s="7"/>
     </row>
     <row r="63" ht="16.5" customHeight="1">
       <c r="A63" s="7"/>
@@ -2371,7 +2377,7 @@
       <c r="I73" s="4"/>
       <c r="J73" s="4"/>
     </row>
-    <row r="74" ht="20.25" customHeight="1">
+    <row r="74" ht="16.5" customHeight="1">
       <c r="A74" s="7"/>
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
@@ -2383,7 +2389,7 @@
       <c r="I74" s="4"/>
       <c r="J74" s="4"/>
     </row>
-    <row r="75" ht="16.5" customHeight="1">
+    <row r="75" ht="20.25" customHeight="1">
       <c r="A75" s="7"/>
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
@@ -2791,7 +2797,7 @@
       <c r="I108" s="4"/>
       <c r="J108" s="4"/>
     </row>
-    <row r="109" ht="47.25" customHeight="1">
+    <row r="109" ht="16.5" customHeight="1">
       <c r="A109" s="7"/>
       <c r="B109" s="7"/>
       <c r="C109" s="7"/>
@@ -2803,7 +2809,7 @@
       <c r="I109" s="4"/>
       <c r="J109" s="4"/>
     </row>
-    <row r="110" ht="16.5" customHeight="1">
+    <row r="110" ht="47.25" customHeight="1">
       <c r="A110" s="7"/>
       <c r="B110" s="7"/>
       <c r="C110" s="7"/>
@@ -2863,7 +2869,7 @@
       <c r="I114" s="4"/>
       <c r="J114" s="4"/>
     </row>
-    <row r="115" ht="24.75" customHeight="1">
+    <row r="115" ht="16.5" customHeight="1">
       <c r="A115" s="7"/>
       <c r="B115" s="7"/>
       <c r="C115" s="7"/>
@@ -2875,7 +2881,7 @@
       <c r="I115" s="4"/>
       <c r="J115" s="4"/>
     </row>
-    <row r="116" ht="16.5" customHeight="1">
+    <row r="116" ht="24.75" customHeight="1">
       <c r="A116" s="7"/>
       <c r="B116" s="7"/>
       <c r="C116" s="7"/>
@@ -3451,7 +3457,7 @@
       <c r="I163" s="4"/>
       <c r="J163" s="4"/>
     </row>
-    <row r="164" ht="42.75" customHeight="1">
+    <row r="164" ht="16.5" customHeight="1">
       <c r="A164" s="7"/>
       <c r="B164" s="7"/>
       <c r="C164" s="7"/>
@@ -3475,7 +3481,7 @@
       <c r="I165" s="4"/>
       <c r="J165" s="4"/>
     </row>
-    <row r="166" ht="16.5" customHeight="1">
+    <row r="166" ht="42.75" customHeight="1">
       <c r="A166" s="7"/>
       <c r="B166" s="7"/>
       <c r="C166" s="7"/>
@@ -3499,7 +3505,7 @@
       <c r="I167" s="4"/>
       <c r="J167" s="4"/>
     </row>
-    <row r="168" ht="58.5" customHeight="1">
+    <row r="168" ht="16.5" customHeight="1">
       <c r="A168" s="7"/>
       <c r="B168" s="7"/>
       <c r="C168" s="7"/>
@@ -3511,7 +3517,7 @@
       <c r="I168" s="4"/>
       <c r="J168" s="4"/>
     </row>
-    <row r="169" ht="47.25" customHeight="1">
+    <row r="169" ht="58.5" customHeight="1">
       <c r="A169" s="7"/>
       <c r="B169" s="7"/>
       <c r="C169" s="7"/>
@@ -3535,7 +3541,7 @@
       <c r="I170" s="4"/>
       <c r="J170" s="4"/>
     </row>
-    <row r="171" ht="24.75" customHeight="1">
+    <row r="171" ht="47.25" customHeight="1">
       <c r="A171" s="7"/>
       <c r="B171" s="7"/>
       <c r="C171" s="7"/>
@@ -3571,7 +3577,7 @@
       <c r="I173" s="4"/>
       <c r="J173" s="4"/>
     </row>
-    <row r="174" ht="36" customHeight="1">
+    <row r="174" ht="24.75" customHeight="1">
       <c r="A174" s="7"/>
       <c r="B174" s="7"/>
       <c r="C174" s="7"/>
@@ -3583,7 +3589,7 @@
       <c r="I174" s="4"/>
       <c r="J174" s="4"/>
     </row>
-    <row r="175" ht="24.75" customHeight="1">
+    <row r="175" ht="36" customHeight="1">
       <c r="A175" s="7"/>
       <c r="B175" s="7"/>
       <c r="C175" s="7"/>
@@ -3595,7 +3601,7 @@
       <c r="I175" s="4"/>
       <c r="J175" s="4"/>
     </row>
-    <row r="176" ht="16.5" customHeight="1">
+    <row r="176" ht="24.75" customHeight="1">
       <c r="A176" s="7"/>
       <c r="B176" s="7"/>
       <c r="C176" s="7"/>
@@ -3979,7 +3985,7 @@
       <c r="I207" s="4"/>
       <c r="J207" s="4"/>
     </row>
-    <row r="208" ht="36" customHeight="1">
+    <row r="208" ht="16.5" customHeight="1">
       <c r="A208" s="7"/>
       <c r="B208" s="7"/>
       <c r="C208" s="7"/>
@@ -3991,7 +3997,7 @@
       <c r="I208" s="4"/>
       <c r="J208" s="4"/>
     </row>
-    <row r="209" ht="16.5" customHeight="1">
+    <row r="209" ht="36" customHeight="1">
       <c r="A209" s="7"/>
       <c r="B209" s="7"/>
       <c r="C209" s="7"/>
@@ -4003,7 +4009,7 @@
       <c r="I209" s="4"/>
       <c r="J209" s="4"/>
     </row>
-    <row r="210" ht="36" customHeight="1">
+    <row r="210" ht="16.5" customHeight="1">
       <c r="A210" s="7"/>
       <c r="B210" s="7"/>
       <c r="C210" s="7"/>
@@ -4015,7 +4021,7 @@
       <c r="I210" s="4"/>
       <c r="J210" s="4"/>
     </row>
-    <row r="211" ht="16.5" customHeight="1">
+    <row r="211" ht="36" customHeight="1">
       <c r="A211" s="7"/>
       <c r="B211" s="7"/>
       <c r="C211" s="7"/>
@@ -4111,19 +4117,19 @@
       <c r="I218" s="4"/>
       <c r="J218" s="4"/>
     </row>
-    <row r="219" ht="33.75" customHeight="1">
+    <row r="219" ht="16.5" customHeight="1">
       <c r="A219" s="7"/>
       <c r="B219" s="7"/>
       <c r="C219" s="7"/>
       <c r="D219" s="7"/>
       <c r="E219" s="7"/>
-      <c r="F219" s="7"/>
-      <c r="G219" s="7"/>
-      <c r="H219" s="7"/>
-      <c r="I219" s="7"/>
-      <c r="J219" s="7"/>
-    </row>
-    <row r="220" ht="16.5" customHeight="1">
+      <c r="F219" s="4"/>
+      <c r="G219" s="4"/>
+      <c r="H219" s="4"/>
+      <c r="I219" s="4"/>
+      <c r="J219" s="4"/>
+    </row>
+    <row r="220" ht="33.75" customHeight="1">
       <c r="A220" s="7"/>
       <c r="B220" s="7"/>
       <c r="C220" s="7"/>
@@ -4135,7 +4141,7 @@
       <c r="I220" s="7"/>
       <c r="J220" s="7"/>
     </row>
-    <row r="221" ht="23.25" customHeight="1">
+    <row r="221" ht="16.5" customHeight="1">
       <c r="A221" s="7"/>
       <c r="B221" s="7"/>
       <c r="C221" s="7"/>
@@ -4147,7 +4153,7 @@
       <c r="I221" s="7"/>
       <c r="J221" s="7"/>
     </row>
-    <row r="222" ht="16.5" customHeight="1">
+    <row r="222" ht="23.25" customHeight="1">
       <c r="A222" s="7"/>
       <c r="B222" s="7"/>
       <c r="C222" s="7"/>
@@ -4171,7 +4177,7 @@
       <c r="I223" s="7"/>
       <c r="J223" s="7"/>
     </row>
-    <row r="224" ht="23.25" customHeight="1">
+    <row r="224" ht="16.5" customHeight="1">
       <c r="A224" s="7"/>
       <c r="B224" s="7"/>
       <c r="C224" s="7"/>
@@ -4183,7 +4189,7 @@
       <c r="I224" s="7"/>
       <c r="J224" s="7"/>
     </row>
-    <row r="225" ht="16.5" customHeight="1">
+    <row r="225" ht="23.25" customHeight="1">
       <c r="A225" s="7"/>
       <c r="B225" s="7"/>
       <c r="C225" s="7"/>
@@ -4213,7 +4219,7 @@
       <c r="C227" s="7"/>
       <c r="D227" s="7"/>
       <c r="E227" s="7"/>
-      <c r="F227" s="8"/>
+      <c r="F227" s="7"/>
       <c r="G227" s="7"/>
       <c r="H227" s="7"/>
       <c r="I227" s="7"/>
@@ -4231,19 +4237,19 @@
       <c r="I228" s="7"/>
       <c r="J228" s="7"/>
     </row>
-    <row r="229" ht="44.25" customHeight="1">
+    <row r="229" ht="16.5" customHeight="1">
       <c r="A229" s="7"/>
       <c r="B229" s="7"/>
       <c r="C229" s="7"/>
       <c r="D229" s="7"/>
       <c r="E229" s="7"/>
-      <c r="F229" s="7"/>
+      <c r="F229" s="8"/>
       <c r="G229" s="7"/>
       <c r="H229" s="7"/>
       <c r="I229" s="7"/>
       <c r="J229" s="7"/>
     </row>
-    <row r="230" ht="16.5" customHeight="1">
+    <row r="230" ht="44.25" customHeight="1">
       <c r="A230" s="7"/>
       <c r="B230" s="7"/>
       <c r="C230" s="7"/>
@@ -4267,7 +4273,7 @@
       <c r="I231" s="7"/>
       <c r="J231" s="7"/>
     </row>
-    <row r="232" ht="65.25" customHeight="1">
+    <row r="232" ht="16.5" customHeight="1">
       <c r="A232" s="7"/>
       <c r="B232" s="7"/>
       <c r="C232" s="7"/>
@@ -4279,7 +4285,7 @@
       <c r="I232" s="7"/>
       <c r="J232" s="7"/>
     </row>
-    <row r="233" ht="16.5" customHeight="1">
+    <row r="233" ht="65.25" customHeight="1">
       <c r="A233" s="7"/>
       <c r="B233" s="7"/>
       <c r="C233" s="7"/>
@@ -4327,7 +4333,7 @@
       <c r="I236" s="7"/>
       <c r="J236" s="7"/>
     </row>
-    <row r="237" ht="33.75" customHeight="1">
+    <row r="237" ht="16.5" customHeight="1">
       <c r="A237" s="7"/>
       <c r="B237" s="7"/>
       <c r="C237" s="7"/>
@@ -4339,7 +4345,7 @@
       <c r="I237" s="7"/>
       <c r="J237" s="7"/>
     </row>
-    <row r="238" ht="16.5" customHeight="1">
+    <row r="238" ht="33.75" customHeight="1">
       <c r="A238" s="7"/>
       <c r="B238" s="7"/>
       <c r="C238" s="7"/>
@@ -4471,7 +4477,7 @@
       <c r="I248" s="7"/>
       <c r="J248" s="7"/>
     </row>
-    <row r="249" ht="23.25" customHeight="1">
+    <row r="249" ht="16.5" customHeight="1">
       <c r="A249" s="7"/>
       <c r="B249" s="7"/>
       <c r="C249" s="7"/>
@@ -4483,7 +4489,7 @@
       <c r="I249" s="7"/>
       <c r="J249" s="7"/>
     </row>
-    <row r="250" ht="16.5" customHeight="1">
+    <row r="250" ht="23.25" customHeight="1">
       <c r="A250" s="7"/>
       <c r="B250" s="7"/>
       <c r="C250" s="7"/>
@@ -4675,7 +4681,7 @@
       <c r="I265" s="7"/>
       <c r="J265" s="7"/>
     </row>
-    <row r="266" ht="23.25" customHeight="1">
+    <row r="266" ht="16.5" customHeight="1">
       <c r="A266" s="7"/>
       <c r="B266" s="7"/>
       <c r="C266" s="7"/>
@@ -4687,7 +4693,7 @@
       <c r="I266" s="7"/>
       <c r="J266" s="7"/>
     </row>
-    <row r="267" ht="16.5" customHeight="1">
+    <row r="267" ht="23.25" customHeight="1">
       <c r="A267" s="7"/>
       <c r="B267" s="7"/>
       <c r="C267" s="7"/>
@@ -4723,7 +4729,7 @@
       <c r="I269" s="7"/>
       <c r="J269" s="7"/>
     </row>
-    <row r="270" ht="33.75" customHeight="1">
+    <row r="270" ht="16.5" customHeight="1">
       <c r="A270" s="7"/>
       <c r="B270" s="7"/>
       <c r="C270" s="7"/>
@@ -4735,7 +4741,7 @@
       <c r="I270" s="7"/>
       <c r="J270" s="7"/>
     </row>
-    <row r="271" ht="16.5" customHeight="1">
+    <row r="271" ht="33.75" customHeight="1">
       <c r="A271" s="7"/>
       <c r="B271" s="7"/>
       <c r="C271" s="7"/>
@@ -4747,7 +4753,7 @@
       <c r="I271" s="7"/>
       <c r="J271" s="7"/>
     </row>
-    <row r="272" ht="23.25" customHeight="1">
+    <row r="272" ht="16.5" customHeight="1">
       <c r="A272" s="7"/>
       <c r="B272" s="7"/>
       <c r="C272" s="7"/>
@@ -4759,7 +4765,7 @@
       <c r="I272" s="7"/>
       <c r="J272" s="7"/>
     </row>
-    <row r="273" ht="16.5" customHeight="1">
+    <row r="273" ht="23.25" customHeight="1">
       <c r="A273" s="7"/>
       <c r="B273" s="7"/>
       <c r="C273" s="7"/>
@@ -4843,7 +4849,7 @@
       <c r="I279" s="7"/>
       <c r="J279" s="7"/>
     </row>
-    <row r="280" ht="33.75" customHeight="1">
+    <row r="280" ht="16.5" customHeight="1">
       <c r="A280" s="7"/>
       <c r="B280" s="7"/>
       <c r="C280" s="7"/>
@@ -4879,7 +4885,7 @@
       <c r="I282" s="7"/>
       <c r="J282" s="7"/>
     </row>
-    <row r="283" ht="16.5" customHeight="1">
+    <row r="283" ht="33.75" customHeight="1">
       <c r="A283" s="7"/>
       <c r="B283" s="7"/>
       <c r="C283" s="7"/>
@@ -4891,7 +4897,7 @@
       <c r="I283" s="7"/>
       <c r="J283" s="7"/>
     </row>
-    <row r="284" ht="23.25" customHeight="1">
+    <row r="284" ht="16.5" customHeight="1">
       <c r="A284" s="7"/>
       <c r="B284" s="7"/>
       <c r="C284" s="7"/>
@@ -4963,7 +4969,7 @@
       <c r="I289" s="7"/>
       <c r="J289" s="7"/>
     </row>
-    <row r="290" ht="16.5" customHeight="1">
+    <row r="290" ht="23.25" customHeight="1">
       <c r="A290" s="7"/>
       <c r="B290" s="7"/>
       <c r="C290" s="7"/>
@@ -5533,7 +5539,7 @@
       <c r="C337" s="7"/>
       <c r="D337" s="7"/>
       <c r="E337" s="7"/>
-      <c r="F337" s="8"/>
+      <c r="F337" s="7"/>
       <c r="G337" s="7"/>
       <c r="H337" s="7"/>
       <c r="I337" s="7"/>
@@ -5545,7 +5551,7 @@
       <c r="C338" s="7"/>
       <c r="D338" s="7"/>
       <c r="E338" s="7"/>
-      <c r="F338" s="7"/>
+      <c r="F338" s="8"/>
       <c r="G338" s="7"/>
       <c r="H338" s="7"/>
       <c r="I338" s="7"/>
@@ -5563,7 +5569,7 @@
       <c r="I339" s="7"/>
       <c r="J339" s="7"/>
     </row>
-    <row r="340" ht="33.75" customHeight="1">
+    <row r="340" ht="16.5" customHeight="1">
       <c r="A340" s="7"/>
       <c r="B340" s="7"/>
       <c r="C340" s="7"/>
@@ -5575,26 +5581,26 @@
       <c r="I340" s="7"/>
       <c r="J340" s="7"/>
     </row>
-    <row r="341" ht="16.5" customHeight="1">
+    <row r="341" ht="33.75" customHeight="1">
       <c r="A341" s="7"/>
       <c r="B341" s="7"/>
       <c r="C341" s="7"/>
       <c r="D341" s="7"/>
       <c r="E341" s="7"/>
-      <c r="F341" s="8"/>
+      <c r="F341" s="7"/>
       <c r="G341" s="7"/>
       <c r="H341" s="7"/>
       <c r="I341" s="7"/>
       <c r="J341" s="7"/>
     </row>
-    <row r="342" ht="33.75" customHeight="1">
+    <row r="342" ht="16.5" customHeight="1">
       <c r="A342" s="7"/>
       <c r="B342" s="7"/>
       <c r="C342" s="7"/>
       <c r="D342" s="7"/>
       <c r="E342" s="7"/>
-      <c r="F342" s="7"/>
-      <c r="G342" s="8"/>
+      <c r="F342" s="8"/>
+      <c r="G342" s="7"/>
       <c r="H342" s="7"/>
       <c r="I342" s="7"/>
       <c r="J342" s="7"/>
@@ -5606,12 +5612,12 @@
       <c r="D343" s="7"/>
       <c r="E343" s="7"/>
       <c r="F343" s="7"/>
-      <c r="G343" s="7"/>
+      <c r="G343" s="8"/>
       <c r="H343" s="7"/>
       <c r="I343" s="7"/>
       <c r="J343" s="7"/>
     </row>
-    <row r="344" ht="16.5" customHeight="1">
+    <row r="344" ht="33.75" customHeight="1">
       <c r="A344" s="7"/>
       <c r="B344" s="7"/>
       <c r="C344" s="7"/>
@@ -5623,7 +5629,7 @@
       <c r="I344" s="7"/>
       <c r="J344" s="7"/>
     </row>
-    <row r="345" ht="44.25" customHeight="1">
+    <row r="345" ht="16.5" customHeight="1">
       <c r="A345" s="7"/>
       <c r="B345" s="7"/>
       <c r="C345" s="7"/>
@@ -5635,7 +5641,7 @@
       <c r="I345" s="7"/>
       <c r="J345" s="7"/>
     </row>
-    <row r="346" ht="23.25" customHeight="1">
+    <row r="346" ht="44.25" customHeight="1">
       <c r="A346" s="7"/>
       <c r="B346" s="7"/>
       <c r="C346" s="7"/>
@@ -5647,7 +5653,7 @@
       <c r="I346" s="7"/>
       <c r="J346" s="7"/>
     </row>
-    <row r="347" ht="16.5" customHeight="1">
+    <row r="347" ht="23.25" customHeight="1">
       <c r="A347" s="7"/>
       <c r="B347" s="7"/>
       <c r="C347" s="7"/>
@@ -5755,7 +5761,7 @@
       <c r="I355" s="7"/>
       <c r="J355" s="7"/>
     </row>
-    <row r="356" ht="23.25" customHeight="1">
+    <row r="356" ht="16.5" customHeight="1">
       <c r="A356" s="7"/>
       <c r="B356" s="7"/>
       <c r="C356" s="7"/>
@@ -5779,7 +5785,7 @@
       <c r="I357" s="7"/>
       <c r="J357" s="7"/>
     </row>
-    <row r="358" ht="16.5" customHeight="1">
+    <row r="358" ht="23.25" customHeight="1">
       <c r="A358" s="7"/>
       <c r="B358" s="7"/>
       <c r="C358" s="7"/>
@@ -5803,6 +5809,18 @@
       <c r="I359" s="7"/>
       <c r="J359" s="7"/>
     </row>
+    <row r="360" ht="16.5" customHeight="1">
+      <c r="A360" s="7"/>
+      <c r="B360" s="7"/>
+      <c r="C360" s="7"/>
+      <c r="D360" s="7"/>
+      <c r="E360" s="7"/>
+      <c r="F360" s="7"/>
+      <c r="G360" s="7"/>
+      <c r="H360" s="7"/>
+      <c r="I360" s="7"/>
+      <c r="J360" s="7"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
Improve plural case ignore  order
</commit_message>
<xml_diff>
--- a/src/test/resources/example.xlsx
+++ b/src/test/resources/example.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="50">
   <si>
     <t>platform</t>
   </si>
@@ -146,6 +146,21 @@
   </si>
   <si>
     <t>one day remaining</t>
+  </si>
+  <si>
+    <t>participant_count</t>
+  </si>
+  <si>
+    <t>%1$d participant</t>
+  </si>
+  <si>
+    <t>%1$d 名成员</t>
+  </si>
+  <si>
+    <t>participant_count.count</t>
+  </si>
+  <si>
+    <t>%1$d participants</t>
   </si>
 </sst>
 </file>
@@ -1646,10 +1661,18 @@
       <c r="J12" s="4"/>
     </row>
     <row r="13" ht="16.5" customHeight="1">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="6"/>
+      <c r="A13" t="s" s="2">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="C13" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="D13" t="s" s="6">
+        <v>47</v>
+      </c>
       <c r="E13" s="2"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
@@ -1658,10 +1681,18 @@
       <c r="J13" s="4"/>
     </row>
     <row r="14" ht="16.5" customHeight="1">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="6"/>
+      <c r="A14" t="s" s="2">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="C14" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="D14" t="s" s="6">
+        <v>47</v>
+      </c>
       <c r="E14" s="2"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>

</xml_diff>

<commit_message>
Fix iOS value with multi placeholder
</commit_message>
<xml_diff>
--- a/src/test/resources/example.xlsx
+++ b/src/test/resources/example.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="48">
   <si>
     <t>platform</t>
   </si>
@@ -97,19 +97,13 @@
     <t>"Agree &amp; Continue"をタップして%1$sと%2$sを受諾してください。</t>
   </si>
   <si>
-    <t>Web</t>
-  </si>
-  <si>
     <t>wallet_transaction_tip</t>
   </si>
   <si>
-    <t>Are you sure you want to transfer %3$s worth %2$s to %1$s ？</t>
+    <t>You have already transferred %3$d to %2$s %1$s. Do you want to transfer it again?</t>
   </si>
   <si>
-    <t>记住密码</t>
-  </si>
-  <si>
-    <t>%1$sへ%2$s相当の%3$sを送金してもよろしいですか？</t>
+    <t>你已经在 %1$s 给 %2$s 转账了 %3$d，确认还要再转一次吗？</t>
   </si>
   <si>
     <t>web_cannot_reached_desc</t>
@@ -1542,20 +1536,18 @@
     </row>
     <row r="7" ht="16.5" customHeight="1">
       <c r="A7" t="s" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s" s="2">
         <v>28</v>
       </c>
-      <c r="B7" t="s" s="2">
+      <c r="C7" t="s" s="2">
         <v>29</v>
       </c>
-      <c r="C7" t="s" s="2">
+      <c r="D7" t="s" s="6">
         <v>30</v>
       </c>
-      <c r="D7" t="s" s="6">
-        <v>31</v>
-      </c>
-      <c r="E7" t="s" s="2">
-        <v>32</v>
-      </c>
+      <c r="E7" s="2"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
@@ -1567,13 +1559,13 @@
         <v>5</v>
       </c>
       <c r="B8" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s" s="6">
         <v>33</v>
-      </c>
-      <c r="C8" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="D8" t="s" s="6">
-        <v>35</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="4"/>
@@ -1587,13 +1579,13 @@
         <v>5</v>
       </c>
       <c r="B9" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="C9" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s" s="6">
         <v>36</v>
-      </c>
-      <c r="C9" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="D9" t="s" s="6">
-        <v>38</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="4"/>
@@ -1607,13 +1599,13 @@
         <v>5</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s" s="2">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D10" t="s" s="6">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="4"/>
@@ -1627,13 +1619,13 @@
         <v>5</v>
       </c>
       <c r="B11" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s" s="6">
         <v>40</v>
-      </c>
-      <c r="C11" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D11" t="s" s="6">
-        <v>42</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="4"/>
@@ -1647,10 +1639,10 @@
         <v>5</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s" s="2">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="2"/>
@@ -1665,13 +1657,13 @@
         <v>5</v>
       </c>
       <c r="B13" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="C13" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D13" t="s" s="6">
         <v>45</v>
-      </c>
-      <c r="C13" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="D13" t="s" s="6">
-        <v>47</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="4"/>
@@ -1685,13 +1677,13 @@
         <v>5</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s" s="2">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D14" t="s" s="6">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="4"/>

</xml_diff>

<commit_message>
Modify parse platform data
</commit_message>
<xml_diff>
--- a/src/test/resources/example.xlsx
+++ b/src/test/resources/example.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
   <si>
     <t>platform</t>
   </si>
@@ -28,7 +28,7 @@
     <t>日文</t>
   </si>
   <si>
-    <t>Mobile</t>
+    <t>Android, iOS</t>
   </si>
   <si>
     <t>error_old_version</t>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>"Agree &amp; Continue"をタップして%1$sと%2$sを受諾してください。</t>
+  </si>
+  <si>
+    <t>Android, iOS, Desktop</t>
   </si>
   <si>
     <t>wallet_transaction_tip</t>
@@ -1536,16 +1539,16 @@
     </row>
     <row r="7" ht="16.5" customHeight="1">
       <c r="A7" t="s" s="2">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s" s="2">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s" s="6">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="4"/>
@@ -1556,16 +1559,16 @@
     </row>
     <row r="8" ht="16.5" customHeight="1">
       <c r="A8" t="s" s="2">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s" s="2">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s" s="6">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="4"/>
@@ -1576,16 +1579,16 @@
     </row>
     <row r="9" ht="16.5" customHeight="1">
       <c r="A9" t="s" s="2">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s" s="6">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="4"/>
@@ -1596,16 +1599,16 @@
     </row>
     <row r="10" ht="16.5" customHeight="1">
       <c r="A10" t="s" s="2">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="D10" t="s" s="6">
         <v>37</v>
-      </c>
-      <c r="C10" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="D10" t="s" s="6">
-        <v>36</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="4"/>
@@ -1616,16 +1619,16 @@
     </row>
     <row r="11" ht="16.5" customHeight="1">
       <c r="A11" t="s" s="2">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D11" t="s" s="6">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="4"/>
@@ -1636,13 +1639,13 @@
     </row>
     <row r="12" ht="16.5" customHeight="1">
       <c r="A12" t="s" s="2">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="2"/>
@@ -1654,16 +1657,16 @@
     </row>
     <row r="13" ht="16.5" customHeight="1">
       <c r="A13" t="s" s="2">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s" s="2">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D13" t="s" s="6">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="4"/>
@@ -1674,16 +1677,16 @@
     </row>
     <row r="14" ht="16.5" customHeight="1">
       <c r="A14" t="s" s="2">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="C14" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="D14" t="s" s="6">
         <v>46</v>
-      </c>
-      <c r="C14" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="D14" t="s" s="6">
-        <v>45</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="4"/>

</xml_diff>

<commit_message>
Use … for Android, ... for iOS
</commit_message>
<xml_diff>
--- a/src/test/resources/example.xlsx
+++ b/src/test/resources/example.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55">
   <si>
     <t>platform</t>
   </si>
@@ -158,6 +158,24 @@
   </si>
   <si>
     <t>%1$d participants</t>
+  </si>
+  <si>
+    <t>Loading</t>
+  </si>
+  <si>
+    <t>Loading…</t>
+  </si>
+  <si>
+    <t>加载中…</t>
+  </si>
+  <si>
+    <t>Preparing</t>
+  </si>
+  <si>
+    <t>Preparing…</t>
+  </si>
+  <si>
+    <t>准备中…</t>
   </si>
 </sst>
 </file>
@@ -1696,10 +1714,18 @@
       <c r="J14" s="4"/>
     </row>
     <row r="15" ht="16.5" customHeight="1">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="6"/>
+      <c r="A15" t="s" s="2">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="C15" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="D15" t="s" s="6">
+        <v>51</v>
+      </c>
       <c r="E15" s="2"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
@@ -1708,10 +1734,18 @@
       <c r="J15" s="4"/>
     </row>
     <row r="16" ht="16.5" customHeight="1">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="6"/>
+      <c r="A16" t="s" s="2">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="C16" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="D16" t="s" s="6">
+        <v>54</v>
+      </c>
       <c r="E16" s="2"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>

</xml_diff>